<commit_message>
fix(fonte-analise): corrige posicao relativa das colunas nos alertas da base fonte-analise. see #13.
</commit_message>
<xml_diff>
--- a/data/fonte_analise.xlsx
+++ b/data/fonte_analise.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -823,7 +823,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4277,7 +4277,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4923,7 +4923,7 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5569,7 +5569,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5641,7 +5641,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5831,7 +5831,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5869,7 +5869,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6169,7 +6169,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6283,7 +6283,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6511,7 +6511,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6663,7 +6663,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6891,7 +6891,7 @@
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -6929,7 +6929,7 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -6967,7 +6967,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7081,7 +7081,7 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7119,7 +7119,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7157,7 +7157,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7533,7 +7533,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7571,7 +7571,7 @@
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7609,7 +7609,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7761,7 +7761,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -7799,7 +7799,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7913,7 +7913,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -7989,7 +7989,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8027,7 +8027,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8065,7 +8065,7 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8141,7 +8141,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8179,7 +8179,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8217,7 +8217,7 @@
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8331,7 +8331,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8369,7 +8369,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8407,7 +8407,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8445,7 +8445,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8521,7 +8521,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8559,7 +8559,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8749,7 +8749,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -8977,7 +8977,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9053,7 +9053,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9129,7 +9129,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9167,7 +9167,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9243,7 +9243,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9281,7 +9281,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9357,7 +9357,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9433,7 +9433,7 @@
       </c>
       <c r="J237" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9471,7 +9471,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9585,7 +9585,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9661,7 +9661,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9699,7 +9699,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9737,7 +9737,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9775,7 +9775,7 @@
       </c>
       <c r="J246" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9813,7 +9813,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9889,7 +9889,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -9927,7 +9927,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10003,7 +10003,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10041,7 +10041,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10079,7 +10079,7 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10117,7 +10117,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10155,7 +10155,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10193,7 +10193,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10231,7 +10231,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10269,7 +10269,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10307,7 +10307,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10345,7 +10345,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10535,7 +10535,7 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10573,7 +10573,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -10611,7 +10611,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10649,7 +10649,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10725,7 +10725,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10763,7 +10763,7 @@
       </c>
       <c r="J272" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -10801,7 +10801,7 @@
       </c>
       <c r="J273" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10877,7 +10877,7 @@
       </c>
       <c r="J275" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10915,7 +10915,7 @@
       </c>
       <c r="J276" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10953,7 +10953,7 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -10991,7 +10991,7 @@
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11029,7 +11029,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11067,7 +11067,7 @@
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11105,7 +11105,7 @@
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11143,7 +11143,7 @@
       </c>
       <c r="J282" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -11219,7 +11219,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11257,7 +11257,7 @@
       </c>
       <c r="J285" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11371,7 +11371,7 @@
       </c>
       <c r="J288" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11409,7 +11409,7 @@
       </c>
       <c r="J289" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11447,7 +11447,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11485,7 +11485,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11523,7 +11523,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11561,7 +11561,7 @@
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11599,7 +11599,7 @@
       </c>
       <c r="J294" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -11637,7 +11637,7 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11675,7 +11675,7 @@
       </c>
       <c r="J296" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -11713,7 +11713,7 @@
       </c>
       <c r="J297" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11751,7 +11751,7 @@
       </c>
       <c r="J298" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11789,7 +11789,7 @@
       </c>
       <c r="J299" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11827,7 +11827,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -11865,7 +11865,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -11903,7 +11903,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11941,7 +11941,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -11979,7 +11979,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12017,7 +12017,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12093,7 +12093,7 @@
       </c>
       <c r="J307" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12131,7 +12131,7 @@
       </c>
       <c r="J308" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12169,7 +12169,7 @@
       </c>
       <c r="J309" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12245,7 +12245,7 @@
       </c>
       <c r="J311" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12283,7 +12283,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12321,7 +12321,7 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12359,7 +12359,7 @@
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12397,7 +12397,7 @@
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12435,7 +12435,7 @@
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12473,7 +12473,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12511,7 +12511,7 @@
       </c>
       <c r="J318" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12549,7 +12549,7 @@
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12587,7 +12587,7 @@
       </c>
       <c r="J320" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -12951,7 +12951,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13027,7 +13027,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -13103,7 +13103,7 @@
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13217,7 +13217,7 @@
       </c>
       <c r="J337" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -13407,7 +13407,7 @@
       </c>
       <c r="J342" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13483,7 +13483,7 @@
       </c>
       <c r="J344" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13521,7 +13521,7 @@
       </c>
       <c r="J345" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13559,7 +13559,7 @@
       </c>
       <c r="J346" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -13597,7 +13597,7 @@
       </c>
       <c r="J347" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13635,7 +13635,7 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13673,7 +13673,7 @@
       </c>
       <c r="J349" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13787,7 +13787,7 @@
       </c>
       <c r="J352" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -13863,7 +13863,7 @@
       </c>
       <c r="J354" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13939,7 +13939,7 @@
       </c>
       <c r="J356" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -13977,7 +13977,7 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="J358" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14053,7 +14053,7 @@
       </c>
       <c r="J359" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -14129,7 +14129,7 @@
       </c>
       <c r="J361" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -14357,7 +14357,7 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14395,7 +14395,7 @@
       </c>
       <c r="J368" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14509,7 +14509,7 @@
       </c>
       <c r="J371" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -14547,7 +14547,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -14619,7 +14619,7 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>ATENCAO</t>
         </is>
       </c>
     </row>
@@ -14657,7 +14657,7 @@
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14733,7 +14733,7 @@
       </c>
       <c r="J377" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14771,7 +14771,7 @@
       </c>
       <c r="J378" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="J379" t="inlineStr">
         <is>
-          <t>VALOR DISCREPANTE</t>
+          <t>RECEITA NAO ESTIMADA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(painel-ldo): atualiza dados e gera bases de dados.
</commit_message>
<xml_diff>
--- a/data/fonte_analise.xlsx
+++ b/data/fonte_analise.xlsx
@@ -9277,11 +9277,11 @@
         <v>300000</v>
       </c>
       <c r="I233" t="n">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>ATENCAO</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -9315,11 +9315,11 @@
         <v>20618556</v>
       </c>
       <c r="I234" t="n">
-        <v>0</v>
+        <v>19613469</v>
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>RECEITA NAO ESTIMADA</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -9353,11 +9353,11 @@
         <v>51898802</v>
       </c>
       <c r="I235" t="n">
-        <v>0</v>
+        <v>63127843</v>
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>RECEITA NAO ESTIMADA</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -10493,11 +10493,11 @@
         <v>1100000</v>
       </c>
       <c r="I265" t="n">
-        <v>0</v>
+        <v>1100000</v>
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>RECEITA NAO ESTIMADA</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -10531,11 +10531,11 @@
         <v>110000</v>
       </c>
       <c r="I266" t="n">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>RECEITA NAO ESTIMADA</t>
+          <t>VALOR DISCREPANTE</t>
         </is>
       </c>
     </row>
@@ -11975,11 +11975,11 @@
         <v>10800000</v>
       </c>
       <c r="I304" t="n">
-        <v>0</v>
+        <v>15800000</v>
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>RECEITA NAO ESTIMADA</t>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>